<commit_message>
Logger now like to smoke crack
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericmiddelhove/Development/rc-car/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB234F6-3CF6-6A48-B589-B6E12EBC4139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58031E93-1BEC-334B-AE41-AA731F69B933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13620" yWindow="6900" windowWidth="28040" windowHeight="17240" xr2:uid="{5FC71DC2-8A43-D349-AF5C-EBEA4452D137}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add emergency button & fix correction sensitivity
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericmiddelhove/Development/rc-car/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58031E93-1BEC-334B-AE41-AA731F69B933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F300F8B1-DAF8-084D-8D25-474CB82088BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13620" yWindow="6900" windowWidth="28040" windowHeight="17240" xr2:uid="{5FC71DC2-8A43-D349-AF5C-EBEA4452D137}"/>
   </bookViews>
@@ -94,13 +94,13 @@
     <t>Power Supply Steering Servo</t>
   </si>
   <si>
-    <t>100Ω Resistor</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
     <t>220Ω Resistor</t>
+  </si>
+  <si>
+    <t>110Ω Resistor</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,10 +616,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>

</xml_diff>